<commit_message>
Added nedmalloc vs system
</commit_message>
<xml_diff>
--- a/ScalingTestResults.xlsx
+++ b/ScalingTestResults.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Bin</t>
   </si>
@@ -83,6 +83,12 @@
   <si>
     <t>umpa improvement</t>
   </si>
+  <si>
+    <t>nedmalloc vs system</t>
+  </si>
+  <si>
+    <t>nedmalloc (umpa) vs system</t>
+  </si>
 </sst>
 </file>
 
@@ -443,25 +449,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105618816"/>
-        <c:axId val="105628800"/>
+        <c:axId val="103520512"/>
+        <c:axId val="103522304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105618816"/>
+        <c:axId val="103520512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105628800"/>
+        <c:crossAx val="103522304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105628800"/>
+        <c:axId val="103522304"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -471,7 +477,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105618816"/>
+        <c:crossAx val="103520512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -484,7 +490,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -701,24 +707,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="105634432"/>
-        <c:axId val="108155264"/>
+        <c:axId val="103821312"/>
+        <c:axId val="103822848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105634432"/>
+        <c:axId val="103821312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108155264"/>
+        <c:crossAx val="103822848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108155264"/>
+        <c:axId val="103822848"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -728,7 +734,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105634432"/>
+        <c:crossAx val="103821312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -741,7 +747,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -760,7 +766,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -836,7 +842,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$20</c:f>
+              <c:f>Sheet1!$J$3:$J$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="18"/>
@@ -903,7 +909,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet1!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -982,7 +988,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$20</c:f>
+              <c:f>Sheet1!$K$3:$K$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1024,24 +1030,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="68450176"/>
-        <c:axId val="68451712"/>
+        <c:axId val="103855616"/>
+        <c:axId val="103857152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68450176"/>
+        <c:axId val="103855616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68451712"/>
+        <c:crossAx val="103857152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68451712"/>
+        <c:axId val="103857152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1055,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68450176"/>
+        <c:crossAx val="103855616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1062,7 +1068,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1081,7 +1087,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>Sheet1!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1157,7 +1163,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$20</c:f>
+              <c:f>Sheet1!$L$3:$L$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1224,7 +1230,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>Sheet1!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1300,7 +1306,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$20</c:f>
+              <c:f>Sheet1!$M$3:$M$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1342,24 +1348,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57064832"/>
-        <c:axId val="68480384"/>
+        <c:axId val="104008704"/>
+        <c:axId val="104047360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57064832"/>
+        <c:axId val="104008704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68480384"/>
+        <c:crossAx val="104047360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68480384"/>
+        <c:axId val="104047360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1367,7 +1373,293 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57064832"/>
+        <c:crossAx val="104008704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-IE"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nedmalloc vs system</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1Kb</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2Kb</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4Kb</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8Kb</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16Kb</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32Kb</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>64Kb</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>128Kb</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>256Kb</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>512Kb</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1Mb</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2Mb</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4Mb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1.8151136647934036</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7159524746425598</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3016691415415798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.4042155531965124</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9361388529636949</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.513028374705029</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.439711767121131</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.6584485034331955</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.0684447001887074</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5007466891247447</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5855722630817608</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.223934954084346</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.3326614378340613</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.068950298233422</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2590638046483313</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.71221013839375269</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.96886530644618774</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.96066075879957258</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.96679021163302148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nedmalloc (umpa) vs system</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>3.7113833449481235</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0625053894221606</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.1471426755230301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0854916974554971</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.4175169893921344</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5166257324931278</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.18299630975139</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.4267744492670094</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6673167804107107</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.1193279205982276</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7524505475974759</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.5991866467841982</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.8154695301356769</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.1331763879984607</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.3630503782772059</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.2118133478934601</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.4226491202293055</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.3767624562582634</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.2456959712189946</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="56916224"/>
+        <c:axId val="56918784"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="56916224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56918784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56918784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56916224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1480,16 +1772,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1503,6 +1795,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1796,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I2" sqref="I2:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1813,7 +2135,7 @@
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1836,10 +2158,10 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -1847,8 +2169,14 @@
       <c r="K1" t="s">
         <v>21</v>
       </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>16</v>
       </c>
@@ -1864,16 +2192,24 @@
       <c r="G2">
         <v>224370.470309</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2">
+        <f>D2/B2</f>
+        <v>1.8151136647934036</v>
+      </c>
+      <c r="I2">
+        <f>D2/G2</f>
+        <v>3.7113833449481235</v>
+      </c>
+      <c r="J2" s="1">
         <f>(B2-G2)/B2</f>
         <v>0.51093339165190044</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <f>B2/G2</f>
         <v>2.0447112579974727</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>32</v>
       </c>
@@ -1889,16 +2225,24 @@
       <c r="G3">
         <v>281392.04071199999</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
+        <f t="shared" ref="H3:H20" si="0">D3/B3</f>
+        <v>1.7159524746425598</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I20" si="1">D3/G3</f>
+        <v>3.0625053894221606</v>
+      </c>
+      <c r="J3" s="1">
         <f>(B3-G3)/B3</f>
         <v>0.43968997391174253</v>
       </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J20" si="0">B3/G3</f>
+      <c r="L3">
+        <f>B3/G3</f>
         <v>1.7847262291224548</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>64</v>
       </c>
@@ -1914,16 +2258,24 @@
       <c r="G4">
         <v>293946.55632199999</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2.3016691415415798</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>4.1471426755230301</v>
+      </c>
+      <c r="J4" s="1">
         <f>(B4-G4)/B4</f>
         <v>0.44499880480931425</v>
       </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
+      <c r="L4">
+        <f>B4/G4</f>
         <v>1.8017979216358675</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>128</v>
       </c>
@@ -1939,16 +2291,24 @@
       <c r="G5">
         <v>271107.10761200002</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>2.4042155531965124</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>5.0854916974554971</v>
+      </c>
+      <c r="J5" s="1">
         <f>(B5-G5)/B5</f>
         <v>0.52724029528954874</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
+      <c r="L5">
+        <f>B5/G5</f>
         <v>2.1152394970135302</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>256</v>
       </c>
@@ -1964,16 +2324,24 @@
       <c r="G6">
         <v>295448.12435200001</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>2.9361388529636949</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>5.4175169893921344</v>
+      </c>
+      <c r="J6" s="1">
         <f>(B6-G6)/B6</f>
         <v>0.45802867647432327</v>
       </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
+      <c r="L6">
+        <f>B6/G6</f>
         <v>1.845116072737423</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>512</v>
       </c>
@@ -1989,16 +2357,24 @@
       <c r="G7">
         <v>320147.103275</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>3.513028374705029</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>6.5166257324931278</v>
+      </c>
+      <c r="J7" s="1">
         <f>(B7-G7)/B7</f>
         <v>0.46091297568488465</v>
       </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
+      <c r="L7">
+        <f>B7/G7</f>
         <v>1.8549880722327772</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2014,16 +2390,24 @@
       <c r="G8">
         <v>300509.46291599999</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>4.439711767121131</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>8.18299630975139</v>
+      </c>
+      <c r="J8" s="1">
         <f>(B8-G8)/B8</f>
         <v>0.45744668590031229</v>
       </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
+      <c r="L8">
+        <f>B8/G8</f>
         <v>1.8431368383757802</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2039,16 +2423,24 @@
       <c r="G9">
         <v>309155.36410300003</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>4.6584485034331955</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>8.4267744492670094</v>
+      </c>
+      <c r="J9" s="1">
         <f>(B9-G9)/B9</f>
         <v>0.44718485922707901</v>
       </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
+      <c r="L9">
+        <f>B9/G9</f>
         <v>1.808922958589458</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2070,24 +2462,32 @@
       <c r="G10">
         <v>460079.52619599999</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>4.0684447001887074</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>6.6673167804107107</v>
+      </c>
+      <c r="J10" s="1">
         <f>(B10-G10)/B10</f>
         <v>0.38979280058475207</v>
       </c>
-      <c r="I10" s="1">
+      <c r="K10" s="1">
         <f>(E10-F10)/E10</f>
         <v>0.15804698884914012</v>
       </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
+      <c r="L10">
+        <f>B10/G10</f>
         <v>1.6387876133849035</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <f>E10/F10</f>
         <v>1.1877147379437563</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2109,24 +2509,32 @@
       <c r="G11">
         <v>1525505.8172840001</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>2.5007466891247447</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>3.1193279205982276</v>
+      </c>
+      <c r="J11" s="1">
         <f>(B11-G11)/B11</f>
         <v>0.19830593230956323</v>
       </c>
-      <c r="I11" s="1">
-        <f t="shared" ref="I11:I20" si="1">(E11-F11)/E11</f>
+      <c r="K11" s="1">
+        <f>(E11-F11)/E11</f>
         <v>0.34566686375982419</v>
       </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
+      <c r="L11">
+        <f>B11/G11</f>
         <v>1.2473586125950185</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <f>E11/F11</f>
         <v>1.5282735117864268</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2148,24 +2556,32 @@
       <c r="G12">
         <v>2093524.1692649999</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>2.5855722630817608</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>2.7524505475974759</v>
+      </c>
+      <c r="J12" s="1">
         <f>(B12-G12)/B12</f>
         <v>6.062898556392865E-2</v>
       </c>
-      <c r="I12" s="1">
-        <f t="shared" si="1"/>
+      <c r="K12" s="1">
+        <f>(E12-F12)/E12</f>
         <v>0.48683344070115159</v>
       </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
+      <c r="L12">
+        <f>B12/G12</f>
         <v>1.0645421081044595</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <f>E12/F12</f>
         <v>1.9486850455850506</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2187,24 +2603,32 @@
       <c r="G13">
         <v>2673664.4183009998</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>3.223934954084346</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>3.5991866467841982</v>
+      </c>
+      <c r="J13" s="1">
         <f>(B13-G13)/B13</f>
         <v>0.10426013694931105</v>
       </c>
-      <c r="I13" s="1">
-        <f t="shared" si="1"/>
+      <c r="K13" s="1">
+        <f>(E13-F13)/E13</f>
         <v>0.59266798641547835</v>
       </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
+      <c r="L13">
+        <f>B13/G13</f>
         <v>1.1163955532739431</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <f>E13/F13</f>
         <v>2.4549997708257703</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2226,24 +2650,32 @@
       <c r="G14">
         <v>3384521.5494070002</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>4.3326614378340613</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>4.8154695301356769</v>
+      </c>
+      <c r="J14" s="1">
         <f>(B14-G14)/B14</f>
         <v>0.10026189331697682</v>
       </c>
-      <c r="I14" s="1">
-        <f t="shared" si="1"/>
+      <c r="K14" s="1">
+        <f>(E14-F14)/E14</f>
         <v>0.72505750961793591</v>
       </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
+      <c r="L14">
+        <f>B14/G14</f>
         <v>1.1114345303063828</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <f>E14/F14</f>
         <v>3.6371242531861312</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2265,24 +2697,32 @@
       <c r="G15">
         <v>6081657.820359</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>4.068950298233422</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>4.1331763879984607</v>
+      </c>
+      <c r="J15" s="1">
         <f>(B15-G15)/B15</f>
         <v>1.5539160136386137E-2</v>
       </c>
-      <c r="I15" s="1">
-        <f t="shared" si="1"/>
+      <c r="K15" s="1">
+        <f>(E15-F15)/E15</f>
         <v>0.78391590154877799</v>
       </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
+      <c r="L15">
+        <f>B15/G15</f>
         <v>1.0157844370310747</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <f>E15/F15</f>
         <v>4.6278278094847209</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2304,24 +2744,32 @@
       <c r="G16">
         <v>11614339.118494</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>1.2590638046483313</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>3.3630503782772059</v>
+      </c>
+      <c r="J16" s="1">
         <f>(B16-G16)/B16</f>
         <v>0.62561851205651176</v>
       </c>
-      <c r="I16" s="1">
-        <f t="shared" si="1"/>
+      <c r="K16" s="1">
+        <f>(E16-F16)/E16</f>
         <v>0.81935631846544199</v>
       </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
+      <c r="L16">
+        <f>B16/G16</f>
         <v>2.6710722410263696</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <f>E16/F16</f>
         <v>5.5357596319176832</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2343,24 +2791,32 @@
       <c r="G17">
         <v>36878942.216252998</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.71221013839375269</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>3.2118133478934601</v>
+      </c>
+      <c r="J17" s="1">
         <f>(B17-G17)/B17</f>
         <v>0.77825294895767472</v>
       </c>
-      <c r="I17" s="1">
-        <f t="shared" si="1"/>
+      <c r="K17" s="1">
+        <f>(E17-F17)/E17</f>
         <v>0.83995150259978391</v>
       </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
+      <c r="L17">
+        <f>B17/G17</f>
         <v>4.5096428353815092</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <f>E17/F17</f>
         <v>6.2481061443482826</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2382,24 +2838,32 @@
       <c r="G18">
         <v>75672211.440097004</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0.96886530644618774</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>5.4226491202293055</v>
+      </c>
+      <c r="J18" s="1">
         <f>(B18-G18)/B18</f>
         <v>0.82132989154105218</v>
       </c>
-      <c r="I18" s="1">
-        <f t="shared" si="1"/>
+      <c r="K18" s="1">
+        <f>(E18-F18)/E18</f>
         <v>0.85670238236800778</v>
       </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
+      <c r="L18">
+        <f>B18/G18</f>
         <v>5.5969071078823767</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <f>E18/F18</f>
         <v>6.9784830796568897</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2421,24 +2885,32 @@
       <c r="G19">
         <v>128732828.44889399</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>0.96066075879957258</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>6.3767624562582634</v>
+      </c>
+      <c r="J19" s="1">
         <f>(B19-G19)/B19</f>
         <v>0.84934976559197939</v>
       </c>
-      <c r="I19" s="1">
-        <f t="shared" si="1"/>
+      <c r="K19" s="1">
+        <f>(E19-F19)/E19</f>
         <v>0.8573489685549065</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
+      <c r="L19">
+        <f>B19/G19</f>
         <v>6.6378920944231883</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <f>E19/F19</f>
         <v>7.0101140515405334</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2460,19 +2932,27 @@
       <c r="G20">
         <v>264084125.044366</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0.96679021163302148</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>6.2456959712189946</v>
+      </c>
+      <c r="J20" s="1">
         <f>(B20-G20)/B20</f>
         <v>0.84520696875286272</v>
       </c>
-      <c r="I20" s="1">
-        <f t="shared" si="1"/>
+      <c r="K20" s="1">
+        <f>(E20-F20)/E20</f>
         <v>0.83706183026305137</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
+      <c r="L20">
+        <f>B20/G20</f>
         <v>6.4602391460597071</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <f>E20/F20</f>
         <v>6.1372973663226036</v>
       </c>

</xml_diff>